<commit_message>
Updates + python file
</commit_message>
<xml_diff>
--- a/MayResults.xlsx
+++ b/MayResults.xlsx
@@ -1,31 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Maths\G2 Maths\DataTest\20232024Grade2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9252CB3F-A13C-4457-A192-1A94B02BE16C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D56A57B5-B8AE-4144-9589-1FEC9BEF477E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t>Names</t>
   </si>
@@ -91,13 +102,19 @@
   </si>
   <si>
     <t>Amy Ke</t>
+  </si>
+  <si>
+    <t>Overall</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,13 +122,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -123,14 +159,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="0" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -408,22 +450,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD16"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -445,86 +488,526 @@
       <c r="G1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B2" s="1">
+        <f>2/5</f>
+        <v>0.4</v>
+      </c>
+      <c r="C2" s="1">
+        <f>4/5</f>
+        <v>0.8</v>
+      </c>
+      <c r="D2" s="1">
+        <f>5/5</f>
+        <v>1</v>
+      </c>
+      <c r="E2" s="1">
+        <f>5/5</f>
+        <v>1</v>
+      </c>
+      <c r="F2" s="1">
+        <f>2/5</f>
+        <v>0.4</v>
+      </c>
+      <c r="G2" s="1">
+        <f>2/5</f>
+        <v>0.4</v>
+      </c>
+      <c r="H2" s="1">
+        <f>20/30</f>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B3" s="1">
+        <f>5/5</f>
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <f>5/5</f>
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <f>5/5</f>
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
+        <f>5/5</f>
+        <v>1</v>
+      </c>
+      <c r="F3" s="1">
+        <f>4/5</f>
+        <v>0.8</v>
+      </c>
+      <c r="G3" s="1">
+        <f>5/5</f>
+        <v>1</v>
+      </c>
+      <c r="H3" s="1">
+        <f>29/30</f>
+        <v>0.96666666666666667</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B4" s="1">
+        <f>5/5</f>
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
+        <f>4/5</f>
+        <v>0.8</v>
+      </c>
+      <c r="D4" s="1">
+        <f>5/5</f>
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <f>5/5</f>
+        <v>1</v>
+      </c>
+      <c r="F4" s="1">
+        <f>4/5</f>
+        <v>0.8</v>
+      </c>
+      <c r="G4" s="1">
+        <f>5/5</f>
+        <v>1</v>
+      </c>
+      <c r="H4" s="1">
+        <f>28/30</f>
+        <v>0.93333333333333335</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B5" s="1">
+        <f>4/5</f>
+        <v>0.8</v>
+      </c>
+      <c r="C5" s="1">
+        <f>4/5</f>
+        <v>0.8</v>
+      </c>
+      <c r="D5" s="1">
+        <f>3/5</f>
+        <v>0.6</v>
+      </c>
+      <c r="E5" s="1">
+        <f>5/5</f>
+        <v>1</v>
+      </c>
+      <c r="F5" s="1">
+        <f>4/5</f>
+        <v>0.8</v>
+      </c>
+      <c r="G5" s="1">
+        <f>5/5</f>
+        <v>1</v>
+      </c>
+      <c r="H5" s="1">
+        <f>25/30</f>
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B6" s="1">
+        <f>5/5</f>
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
+        <f>5/5</f>
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <f>4/5</f>
+        <v>0.8</v>
+      </c>
+      <c r="E6" s="1">
+        <f>5/5</f>
+        <v>1</v>
+      </c>
+      <c r="F6" s="1">
+        <f>5/5</f>
+        <v>1</v>
+      </c>
+      <c r="G6" s="1">
+        <f>5/5</f>
+        <v>1</v>
+      </c>
+      <c r="H6" s="1">
+        <f>29/30</f>
+        <v>0.96666666666666667</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B7" s="1">
+        <f>5/5</f>
+        <v>1</v>
+      </c>
+      <c r="C7" s="1">
+        <f>5/5</f>
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <f>5/5</f>
+        <v>1</v>
+      </c>
+      <c r="E7" s="1">
+        <f>5/5</f>
+        <v>1</v>
+      </c>
+      <c r="F7" s="1">
+        <f>4/5</f>
+        <v>0.8</v>
+      </c>
+      <c r="G7" s="1">
+        <f>5/5</f>
+        <v>1</v>
+      </c>
+      <c r="H7" s="1">
+        <f>29/30</f>
+        <v>0.96666666666666667</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B9" s="1">
+        <f>1/5</f>
+        <v>0.2</v>
+      </c>
+      <c r="C9" s="1">
+        <f t="shared" ref="C9:G9" si="0">1/5</f>
+        <v>0.2</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="E9" s="1">
+        <f>2/5</f>
+        <v>0.4</v>
+      </c>
+      <c r="F9" s="1">
+        <f>2/5</f>
+        <v>0.4</v>
+      </c>
+      <c r="G9" s="1">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="H9" s="1">
+        <f>8/30</f>
+        <v>0.26666666666666666</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B10" s="1">
+        <f>4/5</f>
+        <v>0.8</v>
+      </c>
+      <c r="C10" s="1">
+        <f>4/5</f>
+        <v>0.8</v>
+      </c>
+      <c r="D10" s="1">
+        <f>3/5</f>
+        <v>0.6</v>
+      </c>
+      <c r="E10" s="1">
+        <f>5/5</f>
+        <v>1</v>
+      </c>
+      <c r="F10" s="1">
+        <f>4/5</f>
+        <v>0.8</v>
+      </c>
+      <c r="G10" s="1">
+        <f>5/5</f>
+        <v>1</v>
+      </c>
+      <c r="H10" s="1">
+        <f>25/30</f>
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B11" s="1">
+        <f>5/5</f>
+        <v>1</v>
+      </c>
+      <c r="C11" s="1">
+        <f>4/5</f>
+        <v>0.8</v>
+      </c>
+      <c r="D11" s="1">
+        <f>5/5</f>
+        <v>1</v>
+      </c>
+      <c r="E11" s="1">
+        <f>5/5</f>
+        <v>1</v>
+      </c>
+      <c r="F11" s="1">
+        <f>2/5</f>
+        <v>0.4</v>
+      </c>
+      <c r="G11" s="1">
+        <f>4/5</f>
+        <v>0.8</v>
+      </c>
+      <c r="H11" s="1">
+        <f>25/30</f>
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B12" s="1">
+        <f>0/5</f>
+        <v>0</v>
+      </c>
+      <c r="C12" s="1">
+        <f>0/5</f>
+        <v>0</v>
+      </c>
+      <c r="D12" s="1">
+        <f>3/5</f>
+        <v>0.6</v>
+      </c>
+      <c r="E12" s="1">
+        <f>5/5</f>
+        <v>1</v>
+      </c>
+      <c r="F12" s="1">
+        <f>4/5</f>
+        <v>0.8</v>
+      </c>
+      <c r="G12" s="1">
+        <f>5/5</f>
+        <v>1</v>
+      </c>
+      <c r="H12" s="1">
+        <f>17/30</f>
+        <v>0.56666666666666665</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B13" s="1">
+        <f>0/5</f>
+        <v>0</v>
+      </c>
+      <c r="C13" s="1">
+        <f>2/5</f>
+        <v>0.4</v>
+      </c>
+      <c r="D13" s="1">
+        <f>2/5</f>
+        <v>0.4</v>
+      </c>
+      <c r="E13" s="1">
+        <f>3/5</f>
+        <v>0.6</v>
+      </c>
+      <c r="F13" s="1">
+        <f>2/5</f>
+        <v>0.4</v>
+      </c>
+      <c r="G13" s="1">
+        <f t="shared" ref="G13" si="1">1/5</f>
+        <v>0.2</v>
+      </c>
+      <c r="H13" s="1">
+        <f>10/30</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B14" s="1">
+        <f>2/5</f>
+        <v>0.4</v>
+      </c>
+      <c r="C14" s="1">
+        <f>3/5</f>
+        <v>0.6</v>
+      </c>
+      <c r="D14" s="1">
+        <f>3/5</f>
+        <v>0.6</v>
+      </c>
+      <c r="E14" s="1">
+        <f>4/5</f>
+        <v>0.8</v>
+      </c>
+      <c r="F14" s="1">
+        <f>4/5</f>
+        <v>0.8</v>
+      </c>
+      <c r="G14" s="1">
+        <f>3/5</f>
+        <v>0.6</v>
+      </c>
+      <c r="H14" s="1">
+        <f>19/30</f>
+        <v>0.6333333333333333</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B15" s="1">
+        <f>5/5</f>
+        <v>1</v>
+      </c>
+      <c r="C15" s="1">
+        <f>4/5</f>
+        <v>0.8</v>
+      </c>
+      <c r="D15" s="1">
+        <f>5/5</f>
+        <v>1</v>
+      </c>
+      <c r="E15" s="1">
+        <f>5/5</f>
+        <v>1</v>
+      </c>
+      <c r="F15" s="1">
+        <f>4/5</f>
+        <v>0.8</v>
+      </c>
+      <c r="G15" s="1">
+        <f>5/5</f>
+        <v>1</v>
+      </c>
+      <c r="H15" s="1">
+        <f>28/30</f>
+        <v>0.93333333333333335</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>8</v>
+      </c>
+      <c r="B16" s="1">
+        <f>5/5</f>
+        <v>1</v>
+      </c>
+      <c r="C16" s="1">
+        <f>4/5</f>
+        <v>0.8</v>
+      </c>
+      <c r="D16" s="1">
+        <f>5/5</f>
+        <v>1</v>
+      </c>
+      <c r="E16" s="1">
+        <f>5/5</f>
+        <v>1</v>
+      </c>
+      <c r="F16" s="1">
+        <f>3/5</f>
+        <v>0.6</v>
+      </c>
+      <c r="G16" s="1">
+        <f>5/5</f>
+        <v>1</v>
+      </c>
+      <c r="H16" s="1">
+        <f>27/30</f>
+        <v>0.9</v>
       </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G16">
     <sortCondition ref="A2:A16"/>
   </sortState>
+  <conditionalFormatting sqref="B2:G16">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H16">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>